<commit_message>
Update: learning guide 02 resources
</commit_message>
<xml_diff>
--- a/modulo3/G2.Ventas-mayo-2024.xlsx
+++ b/modulo3/G2.Ventas-mayo-2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evare\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evare\OneDrive\Documentos\Cursos repositorios\diplomado-ciencia-de-datos\modulo3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494BCF57-C337-41FE-8A61-EEC9AD028C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03A30BB-38E9-4094-A536-5DFF086F3212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Venta de figuras mayo 2024</t>
   </si>
@@ -59,74 +59,71 @@
     <t>Red</t>
   </si>
   <si>
-    <t>Frank</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
-    <t>Jo</t>
-  </si>
-  <si>
     <t>Black</t>
   </si>
   <si>
-    <t>Helen</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
-    <t>Mo</t>
-  </si>
-  <si>
     <t>Yellow</t>
   </si>
   <si>
-    <t>Imran</t>
-  </si>
-  <si>
     <t>Brown</t>
   </si>
   <si>
-    <t>Jim</t>
-  </si>
-  <si>
     <t>White</t>
   </si>
   <si>
-    <t>Vana</t>
-  </si>
-  <si>
     <t>Purple</t>
   </si>
   <si>
-    <t>Ivanka</t>
-  </si>
-  <si>
     <t>Indigo</t>
   </si>
   <si>
-    <t>Lea</t>
-  </si>
-  <si>
     <t>Mauve</t>
   </si>
   <si>
-    <t>Kays</t>
-  </si>
-  <si>
     <t>3+</t>
   </si>
   <si>
     <t>1+</t>
+  </si>
+  <si>
+    <t>Cherokee Macias</t>
+  </si>
+  <si>
+    <t>Vladimir Potter</t>
+  </si>
+  <si>
+    <t>David Mckenzie</t>
+  </si>
+  <si>
+    <t>Cassady Leblanc</t>
+  </si>
+  <si>
+    <t>Uriah Knapp</t>
+  </si>
+  <si>
+    <t>Emerald Black</t>
+  </si>
+  <si>
+    <t>Xantha Beck</t>
+  </si>
+  <si>
+    <t>Virginia Holman</t>
+  </si>
+  <si>
+    <t>Zenia Cameron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +137,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +167,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -172,6 +175,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -665,7 +671,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15"/>
@@ -711,8 +717,8 @@
       <c r="D6" s="1">
         <v>45493</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F6">
         <v>441</v>
@@ -723,16 +729,16 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>45490</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F7">
         <v>510</v>
@@ -743,7 +749,7 @@
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -751,8 +757,8 @@
       <c r="D8" s="1">
         <v>45419</v>
       </c>
-      <c r="E8" t="s">
-        <v>12</v>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="F8">
         <v>369</v>
@@ -763,7 +769,7 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -771,8 +777,8 @@
       <c r="D9" s="1">
         <v>45487</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F9">
         <v>178</v>
@@ -789,7 +795,7 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -797,8 +803,8 @@
       <c r="D12" s="1">
         <v>45603</v>
       </c>
-      <c r="E12" t="s">
-        <v>16</v>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F12">
         <v>443</v>
@@ -809,16 +815,16 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1">
         <v>45511</v>
       </c>
-      <c r="E13" t="s">
-        <v>18</v>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F13">
         <v>471</v>
@@ -829,7 +835,7 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -837,8 +843,8 @@
       <c r="D14" s="1">
         <v>45419</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
+      <c r="E14" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="F14">
         <v>369</v>
@@ -849,7 +855,7 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
@@ -857,8 +863,8 @@
       <c r="D15" s="1">
         <v>45329</v>
       </c>
-      <c r="E15" t="s">
-        <v>20</v>
+      <c r="E15" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F15">
         <v>256</v>
@@ -872,7 +878,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -880,8 +886,8 @@
       <c r="D17" s="1">
         <v>45502</v>
       </c>
-      <c r="E17" t="s">
-        <v>22</v>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="F17">
         <v>392</v>
@@ -892,16 +898,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="B18" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1">
         <v>45499</v>
       </c>
-      <c r="E18" t="s">
-        <v>24</v>
+      <c r="E18" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F18">
         <v>181</v>
@@ -912,7 +918,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="B19" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -920,8 +926,8 @@
       <c r="D19" s="1">
         <v>45496</v>
       </c>
-      <c r="E19" t="s">
-        <v>26</v>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F19">
         <v>439</v>

</xml_diff>